<commit_message>
add header in fr with labels
</commit_message>
<xml_diff>
--- a/excelfile1.xlsx
+++ b/excelfile1.xlsx
@@ -16,16 +16,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>last_name</t>
+    <t>nom</t>
+  </si>
+  <si>
+    <t>prénom</t>
   </si>
   <si>
     <t>age</t>
   </si>
   <si>
-    <t>address</t>
+    <t>adresse</t>
   </si>
   <si>
     <t>aitramdane</t>

</xml_diff>

<commit_message>
Adjust the column width
</commit_message>
<xml_diff>
--- a/excelfile1.xlsx
+++ b/excelfile1.xlsx
@@ -56,10 +56,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -85,8 +93,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,18 +397,24 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="70.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
download json format file with url and add django.http
</commit_message>
<xml_diff>
--- a/excelfile1.xlsx
+++ b/excelfile1.xlsx
@@ -56,6 +56,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy hh:mm AM/PM"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -93,11 +96,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -392,7 +396,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -404,7 +408,7 @@
     <col min="4" max="4" width="70.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -417,8 +421,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="F1" s="2">
+        <v>36892.521</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -432,7 +439,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>8</v>
       </c>

</xml_diff>